<commit_message>
Creacion de subdirectorios test y utils
</commit_message>
<xml_diff>
--- a/Pre_Entrega/Pre-entrega.xlsx
+++ b/Pre_Entrega/Pre-entrega.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nowyo\Desktop\Programacion\Cursos\QA_Automation\Entregas\Pre_Entrega\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5222CDB8-7F99-4F73-B3BF-34347705FB00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48245EBB-85AB-4F19-B834-8AFC261B3916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,14 +70,6 @@
     <t>Alta</t>
   </si>
   <si>
-    <t>1. Ingresar a www.saucedemo.com
-2. Iniciar sesion con las credenciales validas.
-3. Verificar que el titulo de la pagina.
-4. Comprobar que exista al menos un producto visible
-5. Validar la presencia de elementos importantes del interfaz (menu,filtro)
-6. Listar por nombre y/o precio</t>
-  </si>
-  <si>
     <t xml:space="preserve">- El titulo de la pagina sea "Swag Labs"
 - Hay al menos un producto visible
 - Los botones del menu y el filtro se muestran correctamente
@@ -89,12 +81,6 @@
 - Se visualizan los botones del menu y el filtro</t>
   </si>
   <si>
-    <t>ok</t>
-  </si>
-  <si>
-    <t>Todo correcto.</t>
-  </si>
-  <si>
     <t>TC-002</t>
   </si>
   <si>
@@ -102,13 +88,6 @@
   </si>
   <si>
     <t>Carrito de compras</t>
-  </si>
-  <si>
-    <t>1. Ingresar a www.saucedemo.com
-2. Iniciar sesion con las credenciales validas.
-3. Elegir un producto y hacer click en "Add to cart".
-4. Observar y hacer click en el icono del carrito
-5. Verificar qeu el producto agregado se muestre en el carrito.</t>
   </si>
   <si>
     <t xml:space="preserve">- El contador del carrito incrementa a 1
@@ -128,6 +107,27 @@
   </si>
   <si>
     <t>Usuario logueado en la web con standard_user</t>
+  </si>
+  <si>
+    <t>1. Ingresar a www.saucedemo.com .
+2. Iniciar sesion con las credenciales validas.
+3. Verificar que el titulo de la pagina.
+4. Comprobar que exista al menos un producto visible.
+5. Validar la presencia de elementos importantes del interfaz (menu,filtro).
+6. Listar por nombre y/o precio.</t>
+  </si>
+  <si>
+    <t>1. Ingresar a www.saucedemo.com .
+2. Iniciar sesion con las credenciales validas.
+3. Elegir un producto y hacer click en "Add to cart".
+4. Observar y hacer click en el icono del carrito .
+5. Verificar que el producto agregado se muestre en el carrito.</t>
+  </si>
+  <si>
+    <t>Todo Ok</t>
+  </si>
+  <si>
+    <t>Ok</t>
   </si>
 </sst>
 </file>
@@ -189,14 +189,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,7 +417,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -435,7 +434,7 @@
     <col min="10" max="10" width="71" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -481,7 +480,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>14</v>
@@ -490,36 +489,36 @@
         <v>15</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="L2" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>14</v>
@@ -528,28 +527,28 @@
         <v>15</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="L3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -563,7 +562,7 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -577,7 +576,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -591,7 +590,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -605,7 +604,7 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -619,7 +618,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -633,7 +632,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -647,7 +646,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -661,7 +660,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -675,7 +674,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -689,7 +688,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -703,7 +702,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -717,7 +716,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -731,7 +730,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -745,7 +744,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -759,7 +758,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -773,7 +772,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>

</xml_diff>